<commit_message>
Proceso pruebasorquestador (hacer copia proyecto del servidor y subir a git
</commit_message>
<xml_diff>
--- a/ExcelCedulas/COLPENSIONES.xlsx
+++ b/ExcelCedulas/COLPENSIONES.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\UiPath\Both_Imcorporaciones\ExcelCedulas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12A2A65C-AE03-47A4-A2BF-6D9F02EDCB45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36EA4FC9-EAAB-4BFF-BD90-131B719DD1FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2565" yWindow="1410" windowWidth="15375" windowHeight="7785" xr2:uid="{5AC3F363-BB6A-4B3C-BA52-D21931BE4E78}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{5AC3F363-BB6A-4B3C-BA52-D21931BE4E78}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -32,28 +32,50 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Cedulas</t>
-  </si>
-  <si>
-    <t>libranza</t>
-  </si>
-  <si>
-    <t>Afiliacion</t>
-  </si>
-  <si>
-    <t>cuota parcial</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="11">
+  <si>
+    <t>SANCHEZ SANCHEZ JUAN RUBEN</t>
+  </si>
+  <si>
+    <t>DESEMBOLSADO</t>
+  </si>
+  <si>
+    <t>AFILIACION</t>
+  </si>
+  <si>
+    <t>CEDULA</t>
+  </si>
+  <si>
+    <t>NOMBRE</t>
+  </si>
+  <si>
+    <t>LBZA</t>
+  </si>
+  <si>
+    <t>CUOTA TOTAL</t>
+  </si>
+  <si>
+    <t>CUOTA PARC</t>
+  </si>
+  <si>
+    <t>CUOTA PDTE</t>
+  </si>
+  <si>
+    <t>PLAZO</t>
+  </si>
+  <si>
+    <t>ESTADO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,16 +97,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -107,15 +144,58 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -123,7 +203,18 @@
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -433,144 +524,280 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7459CFB-13AD-4F33-B108-F0ED2FD0FA02}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="3" max="3" width="26" customWidth="1"/>
     <col min="5" max="5" width="11.7109375" customWidth="1"/>
     <col min="6" max="6" width="17.140625" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>991207184000</v>
+      </c>
+      <c r="B2" s="12">
+        <v>12106746</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" s="12">
+        <v>23412</v>
+      </c>
+      <c r="E2" s="3">
+        <v>967000</v>
+      </c>
+      <c r="F2" s="4">
+        <v>15000</v>
+      </c>
+      <c r="G2" s="5">
+        <v>952000</v>
+      </c>
+      <c r="H2" s="2">
+        <v>168</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>991207184000</v>
-      </c>
-      <c r="B2">
-        <v>12106746</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2">
-        <v>23412</v>
-      </c>
-      <c r="F2">
-        <v>100001</v>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>991207184001</v>
+      </c>
+      <c r="B3" s="12">
+        <v>9064131</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="12">
+        <v>23451</v>
+      </c>
+      <c r="E3" s="3">
+        <v>967000</v>
+      </c>
+      <c r="F3" s="4">
+        <v>125000</v>
+      </c>
+      <c r="G3" s="5">
+        <v>827000</v>
+      </c>
+      <c r="H3" s="2">
+        <v>168</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>991207184001</v>
-      </c>
-      <c r="B3">
-        <v>9064131</v>
-      </c>
-      <c r="D3">
-        <v>23451</v>
-      </c>
-      <c r="F3">
-        <v>100002</v>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>991207184002</v>
+      </c>
+      <c r="B4" s="12">
+        <v>2459204</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="12">
+        <v>45645</v>
+      </c>
+      <c r="E4" s="3">
+        <v>967000</v>
+      </c>
+      <c r="F4" s="4">
+        <v>467000</v>
+      </c>
+      <c r="G4" s="5">
+        <v>360000</v>
+      </c>
+      <c r="H4" s="2">
+        <v>168</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>991207184002</v>
-      </c>
-      <c r="B4">
-        <v>2459204</v>
-      </c>
-      <c r="D4">
-        <v>45645</v>
-      </c>
-      <c r="F4">
-        <v>100003</v>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>991207184003</v>
+      </c>
+      <c r="B5" s="12">
+        <v>42877961</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="12">
+        <v>98565</v>
+      </c>
+      <c r="E5" s="3">
+        <v>967000</v>
+      </c>
+      <c r="F5" s="4">
+        <v>360000</v>
+      </c>
+      <c r="G5" s="5">
+        <v>360000</v>
+      </c>
+      <c r="H5" s="2">
+        <v>168</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>991207184003</v>
-      </c>
-      <c r="B5">
-        <v>42877961</v>
-      </c>
-      <c r="D5">
-        <v>98565</v>
-      </c>
-      <c r="F5">
-        <v>100004</v>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>991207184004</v>
+      </c>
+      <c r="B6" s="12">
+        <v>22632374</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="12">
+        <v>23443</v>
+      </c>
+      <c r="E6" s="3">
+        <v>967000</v>
+      </c>
+      <c r="F6" s="4">
+        <v>360000</v>
+      </c>
+      <c r="G6" s="5">
+        <v>360000</v>
+      </c>
+      <c r="H6" s="2">
+        <v>168</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>991207184004</v>
-      </c>
-      <c r="B6">
-        <v>22632374</v>
-      </c>
-      <c r="D6">
-        <v>23443</v>
-      </c>
-      <c r="F6">
-        <v>100005</v>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>991207184005</v>
+      </c>
+      <c r="B7" s="12">
+        <v>41676517</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="12">
+        <v>45651</v>
+      </c>
+      <c r="E7" s="3">
+        <v>967000</v>
+      </c>
+      <c r="F7" s="4">
+        <v>360000</v>
+      </c>
+      <c r="G7" s="5">
+        <v>360000</v>
+      </c>
+      <c r="H7" s="2">
+        <v>168</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>991207184005</v>
-      </c>
-      <c r="B7">
-        <v>41676517</v>
-      </c>
-      <c r="D7">
-        <v>45651</v>
-      </c>
-      <c r="F7">
-        <v>100006</v>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>991207184006</v>
+      </c>
+      <c r="B8" s="12">
+        <v>17321570</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="12">
+        <v>87452</v>
+      </c>
+      <c r="E8" s="3">
+        <v>967000</v>
+      </c>
+      <c r="F8" s="4">
+        <v>360000</v>
+      </c>
+      <c r="G8" s="5">
+        <v>360000</v>
+      </c>
+      <c r="H8" s="2">
+        <v>168</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>991207184006</v>
-      </c>
-      <c r="B8">
-        <v>17321570</v>
-      </c>
-      <c r="D8">
-        <v>87452</v>
-      </c>
-      <c r="F8">
-        <v>100007</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <v>991207184007</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="12">
         <v>51794619</v>
       </c>
-      <c r="D9">
+      <c r="C9" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="12">
         <v>72324</v>
       </c>
-      <c r="F9">
-        <v>100008</v>
+      <c r="E9" s="3">
+        <v>967000</v>
+      </c>
+      <c r="F9" s="4">
+        <v>360000</v>
+      </c>
+      <c r="G9" s="5">
+        <v>360000</v>
+      </c>
+      <c r="H9" s="2">
+        <v>168</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>